<commit_message>
arreglo errores en el back
</commit_message>
<xml_diff>
--- a/Sprint- Backlog.xlsx
+++ b/Sprint- Backlog.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ito\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pato\Documents\GitHub\Doc_PPTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="91">
   <si>
     <t>No Comenzado</t>
   </si>
@@ -214,9 +214,6 @@
     <t>Semana 12</t>
   </si>
   <si>
-    <t xml:space="preserve">Mejoras en Geolocalizacion </t>
-  </si>
-  <si>
     <t xml:space="preserve">Usuarios </t>
   </si>
   <si>
@@ -291,6 +288,12 @@
   <si>
     <t>fernando</t>
   </si>
+  <si>
+    <t>Arreglo de errores</t>
+  </si>
+  <si>
+    <t>modulo junta de vecinos</t>
+  </si>
 </sst>
 </file>
 
@@ -299,7 +302,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -344,6 +347,14 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -867,9 +878,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -884,6 +892,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,6 +939,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1260,6 +1272,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1273,7 +1286,7 @@
             <a:pPr lvl="0">
               <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1066560748"/>
@@ -1319,6 +1332,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1337,7 +1351,7 @@
             <a:pPr lvl="0">
               <a:defRPr sz="1200"/>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1336769584"/>
@@ -1352,6 +1366,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1401,6 +1416,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1620,6 +1636,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1633,7 +1650,7 @@
             <a:pPr lvl="0">
               <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1155326048"/>
@@ -1677,7 +1694,7 @@
             <a:pPr lvl="0">
               <a:defRPr sz="1200"/>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="574951040"/>
@@ -1687,6 +1704,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2385,7 +2403,7 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2440,13 +2458,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>485774</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>857249</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2515,13 +2533,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>1076325</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2582,13 +2600,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2743,13 +2761,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2818,13 +2836,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2893,13 +2911,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2968,13 +2986,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>85726</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3029,13 +3047,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>752474</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>314326</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3104,13 +3122,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>971550</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3171,13 +3189,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3258,13 +3276,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3329,13 +3347,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3400,13 +3418,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3847,11 +3865,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E62" sqref="E62"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3874,22 +3892,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="109" t="s">
+      <c r="B1" s="106"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="107"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="110" t="s">
+      <c r="E1" s="106"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="112"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="111"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -5409,10 +5427,10 @@
         <v>5</v>
       </c>
       <c r="I39" s="43" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="J39" s="81" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="K39" s="44"/>
       <c r="L39" s="5"/>
@@ -5447,10 +5465,10 @@
         <v>3</v>
       </c>
       <c r="I40" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J40" s="69" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="K40" s="39"/>
       <c r="L40" s="5"/>
@@ -5479,13 +5497,13 @@
         <v>0</v>
       </c>
       <c r="G41" s="76">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H41" s="76">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I41" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J41" s="69" t="s">
         <v>18</v>
@@ -5545,28 +5563,24 @@
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="80">
-        <v>0</v>
+    <row r="43" spans="1:26" s="28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="76"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="102"/>
+      <c r="G43" s="76">
+        <v>3</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="C43" s="70"/>
-      <c r="D43" s="80">
-        <v>0</v>
+      <c r="H43" s="76">
+        <v>3</v>
       </c>
-      <c r="G43" s="82">
-        <v>5</v>
+      <c r="I43" s="33" t="s">
+        <v>90</v>
       </c>
-      <c r="H43" s="82">
-        <v>5</v>
+      <c r="J43" s="69" t="s">
+        <v>45</v>
       </c>
-      <c r="I43" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="J43" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="K43" s="23"/>
+      <c r="K43" s="39"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
@@ -5583,23 +5597,28 @@
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
     </row>
-    <row r="44" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D44" s="83">
-        <v>3</v>
-      </c>
-      <c r="E44" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="F44" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="G44" s="83">
+    <row r="44" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="80">
         <v>0</v>
       </c>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="68"/>
-      <c r="K44" s="37"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="70"/>
+      <c r="D44" s="80">
+        <v>0</v>
+      </c>
+      <c r="G44" s="82">
+        <v>5</v>
+      </c>
+      <c r="H44" s="82">
+        <v>5</v>
+      </c>
+      <c r="I44" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="J44" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="K44" s="23"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
@@ -5617,22 +5636,22 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D45" s="84">
-        <v>2</v>
+      <c r="D45" s="83">
+        <v>3</v>
       </c>
-      <c r="E45" s="40" t="s">
-        <v>69</v>
+      <c r="E45" s="34" t="s">
+        <v>67</v>
       </c>
-      <c r="F45" s="64" t="s">
-        <v>72</v>
+      <c r="F45" s="68" t="s">
+        <v>71</v>
       </c>
-      <c r="G45" s="84">
+      <c r="G45" s="83">
         <v>0</v>
       </c>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="69"/>
-      <c r="K45" s="39"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="68"/>
+      <c r="K45" s="37"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
@@ -5651,13 +5670,13 @@
     </row>
     <row r="46" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D46" s="84">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E46" s="40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F46" s="64" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="G46" s="84">
         <v>0</v>
@@ -5687,10 +5706,10 @@
         <v>5</v>
       </c>
       <c r="E47" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F47" s="64" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="G47" s="84">
         <v>0</v>
@@ -5715,23 +5734,23 @@
       <c r="Y47" s="1"/>
       <c r="Z47" s="1"/>
     </row>
-    <row r="48" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D48" s="80">
+    <row r="48" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D48" s="84">
         <v>5</v>
       </c>
-      <c r="E48" s="25" t="s">
-        <v>67</v>
+      <c r="E48" s="40" t="s">
+        <v>70</v>
       </c>
-      <c r="F48" s="65" t="s">
-        <v>34</v>
+      <c r="F48" s="64" t="s">
+        <v>35</v>
       </c>
-      <c r="G48" s="80">
+      <c r="G48" s="84">
         <v>0</v>
       </c>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="70"/>
-      <c r="K48" s="23"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="39"/>
+      <c r="J48" s="69"/>
+      <c r="K48" s="39"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
@@ -5748,28 +5767,23 @@
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
     </row>
-    <row r="49" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="84">
+    <row r="49" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="80">
         <v>5</v>
       </c>
-      <c r="B49" s="40" t="s">
-        <v>82</v>
+      <c r="E49" s="25" t="s">
+        <v>66</v>
       </c>
-      <c r="C49" s="64" t="s">
-        <v>72</v>
+      <c r="F49" s="65" t="s">
+        <v>34</v>
       </c>
-      <c r="D49" s="84">
+      <c r="G49" s="80">
         <v>0</v>
       </c>
-      <c r="E49" s="39"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="84">
-        <v>0</v>
-      </c>
-      <c r="H49" s="39"/>
-      <c r="I49" s="39"/>
-      <c r="J49" s="69"/>
-      <c r="K49" s="39"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="70"/>
+      <c r="K49" s="23"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
@@ -5791,10 +5805,10 @@
         <v>5</v>
       </c>
       <c r="B50" s="40" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C50" s="64" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="D50" s="84">
         <v>0</v>
@@ -5829,10 +5843,10 @@
         <v>5</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C51" s="64" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D51" s="84">
         <v>0</v>
@@ -5862,28 +5876,28 @@
       <c r="Y51" s="1"/>
       <c r="Z51" s="1"/>
     </row>
-    <row r="52" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="80">
+    <row r="52" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="84">
         <v>5</v>
       </c>
-      <c r="B52" s="25" t="s">
-        <v>75</v>
+      <c r="B52" s="40" t="s">
+        <v>73</v>
       </c>
-      <c r="C52" s="65" t="s">
-        <v>76</v>
+      <c r="C52" s="64" t="s">
+        <v>35</v>
       </c>
-      <c r="D52" s="80">
+      <c r="D52" s="84">
         <v>0</v>
       </c>
-      <c r="E52" s="21"/>
-      <c r="F52" s="70"/>
-      <c r="G52" s="80">
+      <c r="E52" s="39"/>
+      <c r="F52" s="85"/>
+      <c r="G52" s="84">
         <v>0</v>
       </c>
-      <c r="H52" s="21"/>
-      <c r="I52" s="21"/>
-      <c r="J52" s="70"/>
-      <c r="K52" s="23"/>
+      <c r="H52" s="39"/>
+      <c r="I52" s="39"/>
+      <c r="J52" s="69"/>
+      <c r="K52" s="39"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
@@ -5900,28 +5914,28 @@
       <c r="Y52" s="1"/>
       <c r="Z52" s="1"/>
     </row>
-    <row r="53" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="83">
+    <row r="53" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="80">
         <v>5</v>
       </c>
-      <c r="B53" s="48" t="s">
-        <v>77</v>
+      <c r="B53" s="25" t="s">
+        <v>74</v>
       </c>
-      <c r="C53" s="66" t="s">
-        <v>18</v>
+      <c r="C53" s="65" t="s">
+        <v>75</v>
       </c>
-      <c r="D53" s="83">
+      <c r="D53" s="80">
         <v>0</v>
       </c>
-      <c r="E53" s="37"/>
-      <c r="F53" s="87"/>
-      <c r="G53" s="83">
+      <c r="E53" s="21"/>
+      <c r="F53" s="70"/>
+      <c r="G53" s="80">
         <v>0</v>
       </c>
-      <c r="H53" s="37"/>
-      <c r="I53" s="37"/>
-      <c r="J53" s="68"/>
-      <c r="K53" s="37"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="70"/>
+      <c r="K53" s="23"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
@@ -5939,27 +5953,27 @@
       <c r="Z53" s="1"/>
     </row>
     <row r="54" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="84">
+      <c r="A54" s="83">
         <v>5</v>
       </c>
-      <c r="B54" s="40" t="s">
-        <v>78</v>
+      <c r="B54" s="48" t="s">
+        <v>76</v>
       </c>
-      <c r="C54" s="64" t="s">
-        <v>35</v>
+      <c r="C54" s="66" t="s">
+        <v>18</v>
       </c>
-      <c r="D54" s="84">
+      <c r="D54" s="83">
         <v>0</v>
       </c>
-      <c r="E54" s="39"/>
-      <c r="F54" s="85"/>
-      <c r="G54" s="84">
+      <c r="E54" s="37"/>
+      <c r="F54" s="87"/>
+      <c r="G54" s="83">
         <v>0</v>
       </c>
-      <c r="H54" s="39"/>
-      <c r="I54" s="39"/>
-      <c r="J54" s="69"/>
-      <c r="K54" s="39"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="68"/>
+      <c r="K54" s="37"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
@@ -5981,10 +5995,10 @@
         <v>5</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C55" s="64" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D55" s="84">
         <v>0</v>
@@ -6014,28 +6028,28 @@
       <c r="Y55" s="1"/>
       <c r="Z55" s="1"/>
     </row>
-    <row r="56" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="80">
+    <row r="56" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="84">
         <v>5</v>
       </c>
-      <c r="B56" s="25" t="s">
-        <v>81</v>
+      <c r="B56" s="40" t="s">
+        <v>78</v>
       </c>
-      <c r="C56" s="65" t="s">
-        <v>45</v>
+      <c r="C56" s="64" t="s">
+        <v>34</v>
       </c>
-      <c r="D56" s="80">
+      <c r="D56" s="84">
         <v>0</v>
       </c>
-      <c r="E56" s="23"/>
-      <c r="F56" s="86"/>
-      <c r="G56" s="80">
+      <c r="E56" s="39"/>
+      <c r="F56" s="85"/>
+      <c r="G56" s="84">
         <v>0</v>
       </c>
-      <c r="H56" s="23"/>
-      <c r="I56" s="23"/>
-      <c r="J56" s="70"/>
-      <c r="K56" s="23"/>
+      <c r="H56" s="39"/>
+      <c r="I56" s="39"/>
+      <c r="J56" s="69"/>
+      <c r="K56" s="39"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
@@ -6052,28 +6066,28 @@
       <c r="Y56" s="1"/>
       <c r="Z56" s="1"/>
     </row>
-    <row r="57" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="83">
+    <row r="57" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="80">
         <v>5</v>
       </c>
-      <c r="B57" s="50" t="s">
+      <c r="B57" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="C57" s="68" t="s">
-        <v>89</v>
+      <c r="C57" s="65" t="s">
+        <v>45</v>
       </c>
-      <c r="D57" s="83">
+      <c r="D57" s="80">
         <v>0</v>
       </c>
-      <c r="E57" s="34"/>
-      <c r="F57" s="68"/>
-      <c r="G57" s="83">
+      <c r="E57" s="23"/>
+      <c r="F57" s="86"/>
+      <c r="G57" s="80">
         <v>0</v>
       </c>
-      <c r="H57" s="34"/>
-      <c r="I57" s="34"/>
-      <c r="J57" s="68"/>
-      <c r="K57" s="37"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
+      <c r="J57" s="70"/>
+      <c r="K57" s="23"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
@@ -6091,27 +6105,27 @@
       <c r="Z57" s="1"/>
     </row>
     <row r="58" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="84">
+      <c r="A58" s="83">
         <v>5</v>
       </c>
-      <c r="B58" s="40" t="s">
-        <v>83</v>
+      <c r="B58" s="50" t="s">
+        <v>79</v>
       </c>
-      <c r="C58" s="64" t="s">
-        <v>35</v>
+      <c r="C58" s="68" t="s">
+        <v>88</v>
       </c>
-      <c r="D58" s="84">
+      <c r="D58" s="83">
         <v>0</v>
       </c>
-      <c r="E58" s="39"/>
-      <c r="F58" s="85"/>
-      <c r="G58" s="84">
+      <c r="E58" s="34"/>
+      <c r="F58" s="68"/>
+      <c r="G58" s="83">
         <v>0</v>
       </c>
-      <c r="H58" s="39"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="69"/>
-      <c r="K58" s="39"/>
+      <c r="H58" s="34"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="68"/>
+      <c r="K58" s="37"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
@@ -6133,10 +6147,10 @@
         <v>5</v>
       </c>
       <c r="B59" s="40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C59" s="64" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D59" s="84">
         <v>0</v>
@@ -6166,28 +6180,28 @@
       <c r="Y59" s="1"/>
       <c r="Z59" s="1"/>
     </row>
-    <row r="60" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="80">
+    <row r="60" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="84">
         <v>5</v>
       </c>
-      <c r="B60" s="25" t="s">
-        <v>85</v>
+      <c r="B60" s="40" t="s">
+        <v>83</v>
       </c>
-      <c r="C60" s="65" t="s">
-        <v>34</v>
+      <c r="C60" s="64" t="s">
+        <v>18</v>
       </c>
-      <c r="D60" s="80">
+      <c r="D60" s="84">
         <v>0</v>
       </c>
-      <c r="E60" s="23"/>
-      <c r="F60" s="86"/>
-      <c r="G60" s="80">
+      <c r="E60" s="39"/>
+      <c r="F60" s="85"/>
+      <c r="G60" s="84">
         <v>0</v>
       </c>
-      <c r="H60" s="23"/>
-      <c r="I60" s="23"/>
-      <c r="J60" s="70"/>
-      <c r="K60" s="23"/>
+      <c r="H60" s="39"/>
+      <c r="I60" s="39"/>
+      <c r="J60" s="69"/>
+      <c r="K60" s="39"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
@@ -6204,28 +6218,28 @@
       <c r="Y60" s="1"/>
       <c r="Z60" s="1"/>
     </row>
-    <row r="61" spans="1:26" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="88">
-        <v>20</v>
+    <row r="61" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="80">
+        <v>5</v>
       </c>
-      <c r="B61" s="46" t="s">
-        <v>86</v>
+      <c r="B61" s="25" t="s">
+        <v>84</v>
       </c>
-      <c r="C61" s="71" t="s">
-        <v>88</v>
+      <c r="C61" s="65" t="s">
+        <v>34</v>
       </c>
-      <c r="D61" s="88">
+      <c r="D61" s="80">
         <v>0</v>
       </c>
-      <c r="E61" s="47"/>
-      <c r="F61" s="89"/>
-      <c r="G61" s="88">
+      <c r="E61" s="23"/>
+      <c r="F61" s="86"/>
+      <c r="G61" s="80">
         <v>0</v>
       </c>
-      <c r="H61" s="47"/>
-      <c r="I61" s="47"/>
-      <c r="J61" s="103"/>
-      <c r="K61" s="47"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="70"/>
+      <c r="K61" s="23"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
@@ -6247,10 +6261,10 @@
         <v>20</v>
       </c>
       <c r="B62" s="46" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C62" s="71" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D62" s="88">
         <v>0</v>
@@ -6280,33 +6294,28 @@
       <c r="Y62" s="1"/>
       <c r="Z62" s="1"/>
     </row>
-    <row r="63" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="105">
-        <f>SUM(A3:A62)</f>
-        <v>100</v>
-      </c>
-      <c r="B63" s="72" t="s">
-        <v>7</v>
-      </c>
-      <c r="C63" s="65"/>
-      <c r="D63" s="90">
-        <f>SUM(D3:D62)</f>
+    <row r="63" spans="1:26" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="88">
         <v>20</v>
       </c>
-      <c r="E63" s="72" t="s">
-        <v>8</v>
+      <c r="B63" s="46" t="s">
+        <v>86</v>
       </c>
-      <c r="F63" s="86"/>
-      <c r="G63" s="104">
-        <f>SUM(G3:G62)</f>
-        <v>110</v>
+      <c r="C63" s="71" t="s">
+        <v>87</v>
       </c>
-      <c r="H63" s="72" t="s">
-        <v>9</v>
+      <c r="D63" s="88">
+        <v>0</v>
       </c>
-      <c r="I63" s="23"/>
-      <c r="J63" s="86"/>
-      <c r="K63" s="1"/>
+      <c r="E63" s="47"/>
+      <c r="F63" s="89"/>
+      <c r="G63" s="88">
+        <v>0</v>
+      </c>
+      <c r="H63" s="47"/>
+      <c r="I63" s="47"/>
+      <c r="J63" s="103"/>
+      <c r="K63" s="47"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
@@ -6323,16 +6332,32 @@
       <c r="Y63" s="1"/>
       <c r="Z63" s="1"/>
     </row>
-    <row r="64" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="12"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
+    <row r="64" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="104">
+        <f>SUM(A3:A63)</f>
+        <v>100</v>
+      </c>
+      <c r="B64" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="65"/>
+      <c r="D64" s="90">
+        <f>SUM(D3:D63)</f>
+        <v>20</v>
+      </c>
+      <c r="E64" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="86"/>
+      <c r="G64" s="112">
+        <f>SUM(G3:G63)</f>
+        <v>110</v>
+      </c>
+      <c r="H64" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="I64" s="23"/>
+      <c r="J64" s="86"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
@@ -6405,17 +6430,16 @@
       <c r="Z66" s="1"/>
     </row>
     <row r="67" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="53"/>
-      <c r="B67" s="49"/>
-      <c r="C67" s="49"/>
-      <c r="D67" s="53"/>
-      <c r="E67" s="54"/>
-      <c r="F67" s="54"/>
-      <c r="G67" s="53"/>
-      <c r="H67" s="54"/>
-      <c r="I67" s="54"/>
-      <c r="J67" s="27"/>
-      <c r="K67" s="54"/>
+      <c r="A67" s="12"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="K67" s="1"/>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
@@ -6434,10 +6458,7 @@
     </row>
     <row r="68" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="53"/>
-      <c r="B68" s="49">
-        <f>SUM(A63+D63+G63)</f>
-        <v>230</v>
-      </c>
+      <c r="B68" s="49"/>
       <c r="C68" s="49"/>
       <c r="D68" s="53"/>
       <c r="E68" s="54"/>
@@ -6464,16 +6485,19 @@
       <c r="Z68" s="1"/>
     </row>
     <row r="69" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="52"/>
-      <c r="B69" s="27"/>
+      <c r="A69" s="53"/>
+      <c r="B69" s="49">
+        <f>SUM(A64+D64+G64)</f>
+        <v>230</v>
+      </c>
       <c r="C69" s="49"/>
-      <c r="D69" s="55"/>
-      <c r="E69" s="27"/>
-      <c r="F69" s="33"/>
-      <c r="G69" s="56"/>
-      <c r="H69" s="57"/>
-      <c r="I69" s="58"/>
-      <c r="J69" s="49"/>
+      <c r="D69" s="53"/>
+      <c r="E69" s="54"/>
+      <c r="F69" s="54"/>
+      <c r="G69" s="53"/>
+      <c r="H69" s="54"/>
+      <c r="I69" s="54"/>
+      <c r="J69" s="27"/>
       <c r="K69" s="54"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
@@ -6495,12 +6519,12 @@
       <c r="A70" s="52"/>
       <c r="B70" s="27"/>
       <c r="C70" s="49"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="33"/>
+      <c r="D70" s="55"/>
+      <c r="E70" s="27"/>
       <c r="F70" s="33"/>
       <c r="G70" s="56"/>
       <c r="H70" s="57"/>
-      <c r="I70" s="49"/>
+      <c r="I70" s="58"/>
       <c r="J70" s="49"/>
       <c r="K70" s="54"/>
       <c r="L70" s="1"/>
@@ -6520,16 +6544,16 @@
       <c r="Z70" s="1"/>
     </row>
     <row r="71" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="59"/>
-      <c r="B71" s="49"/>
+      <c r="A71" s="52"/>
+      <c r="B71" s="27"/>
       <c r="C71" s="49"/>
-      <c r="D71" s="27"/>
-      <c r="E71" s="49"/>
-      <c r="F71" s="54"/>
-      <c r="G71" s="59"/>
-      <c r="H71" s="49"/>
-      <c r="I71" s="54"/>
-      <c r="J71" s="54"/>
+      <c r="D71" s="53"/>
+      <c r="E71" s="33"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="56"/>
+      <c r="H71" s="57"/>
+      <c r="I71" s="49"/>
+      <c r="J71" s="49"/>
       <c r="K71" s="54"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
@@ -6548,16 +6572,16 @@
       <c r="Z71" s="1"/>
     </row>
     <row r="72" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="27"/>
-      <c r="B72" s="27"/>
-      <c r="C72" s="27"/>
+      <c r="A72" s="59"/>
+      <c r="B72" s="49"/>
+      <c r="C72" s="49"/>
       <c r="D72" s="27"/>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="27"/>
-      <c r="H72" s="27"/>
-      <c r="I72" s="27"/>
-      <c r="J72" s="27"/>
+      <c r="E72" s="49"/>
+      <c r="F72" s="54"/>
+      <c r="G72" s="59"/>
+      <c r="H72" s="49"/>
+      <c r="I72" s="54"/>
+      <c r="J72" s="54"/>
       <c r="K72" s="54"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
@@ -6576,15 +6600,15 @@
       <c r="Z72" s="1"/>
     </row>
     <row r="73" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="53"/>
-      <c r="B73" s="49"/>
-      <c r="C73" s="49"/>
-      <c r="D73" s="53"/>
-      <c r="E73" s="54"/>
-      <c r="F73" s="54"/>
-      <c r="G73" s="53"/>
-      <c r="H73" s="54"/>
-      <c r="I73" s="54"/>
+      <c r="A73" s="27"/>
+      <c r="B73" s="27"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="27"/>
+      <c r="E73" s="27"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="27"/>
+      <c r="H73" s="27"/>
+      <c r="I73" s="27"/>
       <c r="J73" s="27"/>
       <c r="K73" s="54"/>
       <c r="L73" s="1"/>
@@ -6632,16 +6656,17 @@
       <c r="Z74" s="1"/>
     </row>
     <row r="75" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="12"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="K75" s="1"/>
+      <c r="A75" s="53"/>
+      <c r="B75" s="49"/>
+      <c r="C75" s="49"/>
+      <c r="D75" s="53"/>
+      <c r="E75" s="54"/>
+      <c r="F75" s="54"/>
+      <c r="G75" s="53"/>
+      <c r="H75" s="54"/>
+      <c r="I75" s="54"/>
+      <c r="J75" s="27"/>
+      <c r="K75" s="54"/>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
@@ -31633,6 +31658,33 @@
       <c r="Y1000" s="1"/>
       <c r="Z1000" s="1"/>
     </row>
+    <row r="1001" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1001" s="12"/>
+      <c r="B1001" s="13"/>
+      <c r="C1001" s="13"/>
+      <c r="D1001" s="12"/>
+      <c r="E1001" s="1"/>
+      <c r="F1001" s="1"/>
+      <c r="G1001" s="12"/>
+      <c r="H1001" s="1"/>
+      <c r="I1001" s="1"/>
+      <c r="K1001" s="1"/>
+      <c r="L1001" s="1"/>
+      <c r="M1001" s="1"/>
+      <c r="N1001" s="1"/>
+      <c r="O1001" s="1"/>
+      <c r="P1001" s="1"/>
+      <c r="Q1001" s="1"/>
+      <c r="R1001" s="1"/>
+      <c r="S1001" s="1"/>
+      <c r="T1001" s="1"/>
+      <c r="U1001" s="1"/>
+      <c r="V1001" s="1"/>
+      <c r="W1001" s="1"/>
+      <c r="X1001" s="1"/>
+      <c r="Y1001" s="1"/>
+      <c r="Z1001" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
@@ -31640,7 +31692,8 @@
     <mergeCell ref="G1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -31876,7 +31929,7 @@
         <v>24</v>
       </c>
       <c r="G4" s="18">
-        <f>SUM('Sprint Backlog'!G39:G43)</f>
+        <f>SUM('Sprint Backlog'!G39:G44)</f>
         <v>20</v>
       </c>
       <c r="H4" s="18">

</xml_diff>